<commit_message>
Review and add trial acronym to other documents
</commit_message>
<xml_diff>
--- a/monitoring-plan/@Monitoring query log.xlsx
+++ b/monitoring-plan/@Monitoring query log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Trauma Study\Monitoring-tools\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Documents/advance-trauma-trial/monitoring-plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DD68A2-F747-4E74-835F-8A9142C40C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C141E7EF-6D23-DC43-8F7C-EB359530AB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9C68889A-3693-45F4-965F-64FC35A3A6B3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20740" windowHeight="11160" xr2:uid="{9C68889A-3693-45F4-965F-64FC35A3A6B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitoring query log" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="ListCat">#REF!</definedName>
     <definedName name="Liststatus">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -99,7 +99,7 @@
     <t>Site Name:</t>
   </si>
   <si>
-    <t>ATLS Study</t>
+    <t>ADVANCE TRAUMA Trial</t>
   </si>
 </sst>
 </file>
@@ -556,20 +556,20 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>18</v>
       </c>
@@ -586,7 +586,7 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
@@ -611,7 +611,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -669,7 +669,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -703,7 +703,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -720,7 +720,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>

</xml_diff>